<commit_message>
added testing data for LTE
</commit_message>
<xml_diff>
--- a/testImages/testing_data.xlsx
+++ b/testImages/testing_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7333D035-36E2-1246-B4B8-C9D55B43BCD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DE8324-E937-F348-B8A4-C77995A71326}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21400" windowHeight="16260" xr2:uid="{FB92F74A-81E7-7845-B700-3DF3187B604C}"/>
+    <workbookView xWindow="360" yWindow="460" windowWidth="21400" windowHeight="16260" xr2:uid="{FB92F74A-81E7-7845-B700-3DF3187B604C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="16">
   <si>
     <t>Start Time</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Std Dev</t>
+  </si>
+  <si>
+    <t>Overall Accuracy</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
   </si>
 </sst>
 </file>
@@ -433,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E780A109-E492-6349-A30A-F2A479B76CF3}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,7 +454,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -468,7 +474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,7 +495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -531,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -552,7 +558,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -573,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -594,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -636,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -657,7 +663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -677,8 +683,15 @@
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1">
+        <f>COUNTIF(E2:E11,"anger")/10</f>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -699,7 +712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -720,7 +733,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -741,7 +754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -762,7 +775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -783,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -804,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -825,7 +838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -846,7 +859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -867,7 +880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -887,8 +900,15 @@
       <c r="F21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="1">
+        <f>COUNTIF(E12:E21,"joy")/10</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -909,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -930,7 +950,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -951,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>11</v>
       </c>
@@ -972,7 +992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -993,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1014,7 +1034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1035,7 +1055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>11</v>
       </c>
@@ -1097,8 +1117,15 @@
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="1">
+        <f>COUNTIF(E22:E31,"sorrow")/10</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -1119,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -1140,7 +1167,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1161,7 +1188,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -1203,7 +1230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1224,7 +1251,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
@@ -1245,7 +1272,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>10</v>
       </c>
@@ -1266,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -1287,7 +1314,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
@@ -1307,24 +1334,38 @@
       <c r="F41" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="1">
+        <f>COUNTIF(E32:E41,"surprised")/10</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D43" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D44" s="2">
         <f>AVERAGE(D2:D41)</f>
         <v>2.9306134259254878E-5</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="1">
+        <f>AVERAGE(H11,H21,H31,H41)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D46" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D47" s="2">
         <f>STDEV(D2:D41)</f>
         <v>4.2173437258695263E-6</v>

</xml_diff>